<commit_message>
Fixed a bunch of stuff. Only left to fix docker-compose.
</commit_message>
<xml_diff>
--- a/backend/default_images_and_spreadsheets/CategoriesSample.xlsx
+++ b/backend/default_images_and_spreadsheets/CategoriesSample.xlsx
@@ -5,22 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Python\PycharmProjects\belmarket\belmarket\default_images_and_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Python\PycharmProjects\belmarket\belmarket\backend\default_images_and_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037BF0CE-1664-43CA-A474-CE74060A301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F051557-2D09-42B1-A661-869BF61FC4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5412" yWindow="2988" windowWidth="12600" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7992" yWindow="2256" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Товары" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -59,6 +70,96 @@
   </si>
   <si>
     <t>Milk.jfif</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Pork</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>Lard</t>
+  </si>
+  <si>
+    <t>Milkshakes</t>
+  </si>
+  <si>
+    <t>Greens</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Drinks</t>
+  </si>
+  <si>
+    <t>Soda</t>
+  </si>
+  <si>
+    <t>Tea</t>
+  </si>
+  <si>
+    <t>Baking</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Pies</t>
+  </si>
+  <si>
+    <t>Chicken.jfif</t>
+  </si>
+  <si>
+    <t>Pork.jpg</t>
+  </si>
+  <si>
+    <t>Cheese.jpg</t>
+  </si>
+  <si>
+    <t>Lard.jpg</t>
+  </si>
+  <si>
+    <t>Milkshakes.jpg</t>
+  </si>
+  <si>
+    <t>Greens.jpg</t>
+  </si>
+  <si>
+    <t>Vegetables.jpg</t>
+  </si>
+  <si>
+    <t>Fruits.jpg</t>
+  </si>
+  <si>
+    <t>Drinks.jpg</t>
+  </si>
+  <si>
+    <t>Soda.jpg</t>
+  </si>
+  <si>
+    <t>Tea.jpg</t>
+  </si>
+  <si>
+    <t>Baking.jpg</t>
+  </si>
+  <si>
+    <t>Bread.jpg</t>
+  </si>
+  <si>
+    <t>Cookies.jpg</t>
+  </si>
+  <si>
+    <t>Pies.jpg</t>
   </si>
 </sst>
 </file>
@@ -421,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,24 +585,189 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>